<commit_message>
update tableau de synthèse
</commit_message>
<xml_diff>
--- a/documents/Ethan-Deglos-BIzouarn-Tableau-de-synthèse-E4.xlsx
+++ b/documents/Ethan-Deglos-BIzouarn-Tableau-de-synthèse-E4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programation_SIO_2nd_annee\PortFolio\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2FFB4CE-B35E-47C9-BBE7-C5FB4D053BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF93A87-DD91-436E-9801-B6DC11B36C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>Option :</t>
   </si>
   <si>
-    <t>Adresse URL du portfolio :</t>
-  </si>
-  <si>
     <t>Compétences mises en œuvre
 Réalisations professionnelles
 (intitulé et liste des documents et productions associés)</t>
@@ -180,6 +177,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Adresse URL du portfolio : https://sopsz.github.io/Portfolio/</t>
   </si>
 </sst>
 </file>
@@ -665,9 +665,48 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -690,45 +729,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1041,8 +1041,8 @@
   </sheetPr>
   <dimension ref="A1:AQ63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1055,124 +1055,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="18"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="20"/>
-      <c r="H3" s="26"/>
+      <c r="A3" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="33"/>
+      <c r="H3" s="39"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="24"/>
+      <c r="A4" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="37"/>
       <c r="F4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="39"/>
+      <c r="A5" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="31"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28"/>
-      <c r="B7" s="36"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="E7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="F7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="G7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="H7" s="15" t="s">
         <v>17</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>18</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -1211,16 +1211,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
+      <c r="A8" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="23"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1259,22 +1259,22 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="C9" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I9"/>
       <c r="J9"/>
@@ -1314,25 +1314,25 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H10" s="12"/>
       <c r="I10"/>
@@ -1373,20 +1373,20 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="12"/>
@@ -1428,16 +1428,16 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
@@ -1480,16 +1480,16 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="34"/>
+      <c r="A13" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="26"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1528,28 +1528,28 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I14"/>
       <c r="J14"/>
@@ -1588,16 +1588,16 @@
       <c r="AQ14"/>
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="34"/>
+      <c r="A15" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1636,28 +1636,28 @@
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I16"/>
       <c r="J16"/>
@@ -1788,6 +1788,11 @@
     <row r="63" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -1795,11 +1800,6 @@
     <mergeCell ref="A15:H15"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -1819,12 +1819,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010086CE4792B3CC0941A62762EF72645E6F" ma:contentTypeVersion="4" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="552e21d6dc657c46617c239f97d2b7c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b58da2c6-99b1-418a-ba38-f77dfe8a9771" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3af089eba0e67a06e887601ee316caa5" ns2:_="">
     <xsd:import namespace="b58da2c6-99b1-418a-ba38-f77dfe8a9771"/>
@@ -1968,6 +1962,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90F4AA83-3EB0-47DD-8E6B-C935DDD5B007}">
   <ds:schemaRefs>
@@ -1977,15 +1977,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7079DFEB-FAF9-4291-AF31-75FF24E8B2F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B752A70C-BA65-477A-AC7D-D3E690F93B8E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2001,4 +1992,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7079DFEB-FAF9-4291-AF31-75FF24E8B2F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>